<commit_message>
A branch for Data Gathering
Will focus oon the data gathering and parameters to be used here
</commit_message>
<xml_diff>
--- a/Raw_Data_Corona_Virus.xlsx
+++ b/Raw_Data_Corona_Virus.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://afonline-my.sharepoint.com/personal/fabian_kallstrom_afconsult_com/Documents/Documents/AFRY/Courses &amp; Skills/Python - Learning Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A547497\PycharmProjects\Python_Test_site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{10D8EE6D-B809-44E4-859F-23447CF9E2D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{A7E1A0EC-C56F-47D5-B90B-C2B95562E69F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0579D96-F63E-49C7-80FB-8D260DC34995}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B11D29B7-BB7D-4F64-A1E9-7BFB1A4CB8B1}"/>
+    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{B11D29B7-BB7D-4F64-A1E9-7BFB1A4CB8B1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Raw_Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -419,7 +419,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,6 +454,18 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
@@ -462,6 +474,18 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
@@ -470,6 +494,18 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4">
+        <v>31</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>33</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
@@ -478,6 +514,18 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5">
+        <v>41</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
@@ -486,6 +534,18 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6">
+        <v>51</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -493,6 +553,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BEFFB8D71F1F84E81A1E69862B58FAE" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090ef84e8672f5641b17f1dd22ba1b0e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="561eae11-18c4-47dc-88fb-bf33d6cec1f5" xmlns:ns4="a0598bb4-3e31-42eb-99e0-e1785d7e0292" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e53bc0461dd0058e7fb1f0777d5d763" ns3:_="" ns4:_="">
     <xsd:import namespace="561eae11-18c4-47dc-88fb-bf33d6cec1f5"/>
@@ -695,22 +770,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A6474F4-0D96-4A3A-A822-C3B20AA6D05F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a0598bb4-3e31-42eb-99e0-e1785d7e0292"/>
+    <ds:schemaRef ds:uri="561eae11-18c4-47dc-88fb-bf33d6cec1f5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B1513B-D3DC-4DAC-A345-31C1BE4FB005}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{451E9562-99F3-40C1-85D9-D61DA9CCE3A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -727,29 +812,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B1513B-D3DC-4DAC-A345-31C1BE4FB005}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A6474F4-0D96-4A3A-A822-C3B20AA6D05F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a0598bb4-3e31-42eb-99e0-e1785d7e0292"/>
-    <ds:schemaRef ds:uri="561eae11-18c4-47dc-88fb-bf33d6cec1f5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added som plots and calculations
To help to finalize the data gathering the plots and calusulations had
to be added to understand what is needed. Not done yet but soon.
</commit_message>
<xml_diff>
--- a/Raw_Data_Corona_Virus.xlsx
+++ b/Raw_Data_Corona_Virus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A547497\PycharmProjects\Python_Test_site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0579D96-F63E-49C7-80FB-8D260DC34995}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0360139F-6FEE-4512-AA93-2C3845D81338}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{B11D29B7-BB7D-4F64-A1E9-7BFB1A4CB8B1}"/>
+    <workbookView xWindow="470" yWindow="50" windowWidth="18040" windowHeight="10150" xr2:uid="{B11D29B7-BB7D-4F64-A1E9-7BFB1A4CB8B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw_Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Country</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Tested</t>
   </si>
   <si>
-    <t>Infected</t>
-  </si>
-  <si>
-    <t>Recovery</t>
-  </si>
-  <si>
     <t>Deaths</t>
   </si>
   <si>
@@ -64,14 +58,64 @@
   </si>
   <si>
     <t>Spain</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>Ref (2020-08-24)</t>
+  </si>
+  <si>
+    <t>Infected Cases</t>
+  </si>
+  <si>
+    <t>Recovery Cases</t>
+  </si>
+  <si>
+    <t>Active Cases</t>
+  </si>
+  <si>
+    <t>Sweden_live</t>
+  </si>
+  <si>
+    <t>USA_live</t>
+  </si>
+  <si>
+    <t>Norway_live</t>
+  </si>
+  <si>
+    <t>India_live</t>
+  </si>
+  <si>
+    <t>Spain_live</t>
+  </si>
+  <si>
+    <t>New Infected</t>
+  </si>
+  <si>
+    <t>New Deaths</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,9 +143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,139 +463,910 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC5402F-CD19-43D9-9A26-E3558030E30D}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <f>SUM(C3:C7)</f>
+        <v>123889358</v>
+      </c>
+      <c r="D2" s="2">
+        <f>SUM(D3:D7)</f>
+        <v>9604497</v>
+      </c>
+      <c r="E2" s="2">
+        <f>SUM(E3:E7)</f>
+        <v>5936696</v>
+      </c>
+      <c r="F2" s="2">
+        <f>SUM(F3:F7)</f>
+        <v>3393168</v>
+      </c>
+      <c r="G2" s="2">
+        <f>SUM(G3:G7)</f>
+        <v>1974633</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1030010</v>
+      </c>
+      <c r="D3" s="2">
+        <v>86721</v>
+      </c>
+      <c r="E3" s="2">
+        <f>D3*0.6</f>
+        <v>52032.6</v>
+      </c>
+      <c r="F3" s="2">
+        <f>D3-E3-G3</f>
+        <v>28875.4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>5813</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C4" s="2">
+        <f>76883479</f>
+        <v>76883479</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5915630</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3217981</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2516535</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1881114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>630903</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10395</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9150</v>
+      </c>
+      <c r="F5" s="2">
+        <v>981</v>
+      </c>
+      <c r="G5" s="2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>36827520</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3170942</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2405047</v>
+      </c>
+      <c r="F6" s="2">
+        <v>707325</v>
+      </c>
+      <c r="G6" s="2">
+        <v>58570</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2">
+        <v>8517446</v>
+      </c>
+      <c r="D7" s="2">
+        <v>420809</v>
+      </c>
+      <c r="E7" s="2">
+        <f>D7*0.6</f>
+        <v>252485.4</v>
+      </c>
+      <c r="F7" s="2">
+        <f>D7-E7-G7</f>
+        <v>139451.6</v>
+      </c>
+      <c r="G7" s="2">
+        <v>28872</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>44067</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>653</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>44068</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2">
+        <v>170</v>
+      </c>
+      <c r="D10" s="2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>44067</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2">
+        <v>38045</v>
+      </c>
+      <c r="D11" s="2">
+        <v>450</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>44068</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <v>37986</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1234</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
         <v>44067</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>21</v>
-      </c>
-      <c r="D3">
-        <v>22</v>
-      </c>
-      <c r="E3">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>44068</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
         <v>44067</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>31</v>
-      </c>
-      <c r="D4">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>33</v>
-      </c>
-      <c r="F4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="2">
+        <v>60975</v>
+      </c>
+      <c r="D15" s="2">
+        <v>848</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>44068</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2">
+        <v>57224</v>
+      </c>
+      <c r="D16" s="2">
+        <v>967</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
         <v>44067</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>41</v>
-      </c>
-      <c r="D5">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>11</v>
-      </c>
-      <c r="F5">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>44067</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>51</v>
-      </c>
-      <c r="D6">
-        <v>11</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>54</v>
-      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2">
+        <v>19382</v>
+      </c>
+      <c r="D17" s="2">
+        <v>34</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>44068</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2">
+        <v>7117</v>
+      </c>
+      <c r="D18" s="2">
+        <v>52</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+    </row>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+    </row>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+    </row>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+    </row>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -559,15 +1377,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BEFFB8D71F1F84E81A1E69862B58FAE" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090ef84e8672f5641b17f1dd22ba1b0e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="561eae11-18c4-47dc-88fb-bf33d6cec1f5" xmlns:ns4="a0598bb4-3e31-42eb-99e0-e1785d7e0292" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e53bc0461dd0058e7fb1f0777d5d763" ns3:_="" ns4:_="">
     <xsd:import namespace="561eae11-18c4-47dc-88fb-bf33d6cec1f5"/>
@@ -770,6 +1579,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A6474F4-0D96-4A3A-A822-C3B20AA6D05F}">
   <ds:schemaRefs>
@@ -788,14 +1606,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B1513B-D3DC-4DAC-A345-31C1BE4FB005}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{451E9562-99F3-40C1-85D9-D61DA9CCE3A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -812,4 +1622,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B1513B-D3DC-4DAC-A345-31C1BE4FB005}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>